<commit_message>
Extra gain added for improved sensitivity
</commit_message>
<xml_diff>
--- a/Amplifier.xlsx
+++ b/Amplifier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\javi_\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\javi_\GitHub\Microwatt_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E2EEF9-0751-4005-87E6-876BDC2C1549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0431C2FA-5F47-4AFB-81E2-3151191C84A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18765" yWindow="3375" windowWidth="17355" windowHeight="17865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2775" yWindow="2130" windowWidth="17355" windowHeight="17865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>V_r</t>
   </si>
@@ -55,19 +55,61 @@
     <t>Gain_1</t>
   </si>
   <si>
-    <t>Vout_1</t>
-  </si>
-  <si>
-    <t>Vout_2</t>
-  </si>
-  <si>
-    <t>Vout_3</t>
-  </si>
-  <si>
     <t>Gain_2</t>
   </si>
   <si>
     <t>Gain_3</t>
+  </si>
+  <si>
+    <t>V_r_max</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>V/V</t>
+  </si>
+  <si>
+    <t>Ohm</t>
+  </si>
+  <si>
+    <t>P_r (mW)</t>
+  </si>
+  <si>
+    <t>V_ldo_1</t>
+  </si>
+  <si>
+    <t>V_ldo_2</t>
+  </si>
+  <si>
+    <t>V_drop_max</t>
+  </si>
+  <si>
+    <t>R_sens (Ohm)</t>
+  </si>
+  <si>
+    <t>P_ldo_2 (mW)</t>
+  </si>
+  <si>
+    <t>Vout_1 (V)</t>
+  </si>
+  <si>
+    <t>Vout_2 (V)</t>
+  </si>
+  <si>
+    <t>Vout_3 (V)</t>
+  </si>
+  <si>
+    <t>V_ref_adc</t>
+  </si>
+  <si>
+    <t>Voltage divider</t>
+  </si>
+  <si>
+    <t>Gain_4</t>
+  </si>
+  <si>
+    <t>Vout_4 (V)</t>
   </si>
 </sst>
 </file>
@@ -86,12 +128,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,10 +154,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,274 +445,531 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C3" s="5"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>1001</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>0</v>
-      </c>
       <c r="B10">
-        <f>A10*B$1/1000/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <f>MIN(3.3,B10*10/33*B$5)</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <f>MIN(3.3,B10*10/33*B$6)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <f>MIN(3.3,B10*10/33*B$7)</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <f>A11*B$1/1000/1000</f>
-        <v>1E-4</v>
-      </c>
-      <c r="C11" s="1">
-        <f>MIN(3.3,B11*10/33*B$5)</f>
-        <v>3.0333333333333334E-2</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" ref="D11:D17" si="0">MIN(3.3,B11*10/33*B$6)</f>
-        <v>3.0606060606060605E-3</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" ref="E11:E17" si="1">MIN(3.3,B11*10/33*B$7)</f>
-        <v>6.0606060606060605E-5</v>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="I11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <f>A12*B$1/1000/1000</f>
-        <v>1E-3</v>
-      </c>
-      <c r="C12" s="1">
-        <f>MIN(3.3,B12*10/33*B$5)</f>
-        <v>0.30333333333333334</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>3.0606060606060605E-2</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="1"/>
-        <v>6.0606060606060606E-4</v>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="I12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>100</v>
-      </c>
-      <c r="B13">
-        <f>A13*B$1/1000/1000</f>
-        <v>0.01</v>
-      </c>
-      <c r="C13" s="1">
-        <f>MIN(3.3,B13*10/33*B$5)</f>
-        <v>3.0333333333333332</v>
-      </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>0.30606060606060603</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="1"/>
-        <v>6.0606060606060606E-3</v>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4">
+        <f>B11-B12-B10</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="I13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B14">
-        <f>A14*B$1/1000/1000</f>
-        <v>0.1</v>
-      </c>
-      <c r="C14" s="1">
-        <f>MIN(3.3,B14*10/33*B$5)</f>
-        <v>3.3</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>3.0606060606060606</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="1"/>
-        <v>6.0606060606060608E-2</v>
-      </c>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="4">
+        <f>3.7/B11</f>
+        <v>0.37</v>
+      </c>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>4.0960000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>100</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f>B19*B$1/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="6">
+        <f>MIN(B$16,C19*B$15*B$5)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <f>MIN(B$16,C19*B$15*B$6)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <f>MIN(B$16,C19*B$15*B$7)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <f>MIN(B$16,C19*B$15*B$8)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <f>A19*(B19/1000000)^2*1000</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <f>(B$11-C19-B$12)*B19/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>100</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f>B20*B$1/1000/1000</f>
+        <v>1E-4</v>
+      </c>
+      <c r="D20" s="6">
+        <f>MIN(B$16,C20*B$15*B$5)</f>
+        <v>3.7037E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <f>MIN(B$16,C20*B$15*B$6)</f>
+        <v>3.7369999999999999E-3</v>
+      </c>
+      <c r="F20" s="1">
+        <f>MIN(B$16,C20*B$15*B$7)</f>
+        <v>4.0699999999999997E-4</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" ref="G20:G26" si="0">MIN(B$16,C20*B$15*B$8)</f>
+        <v>7.3999999999999996E-5</v>
+      </c>
+      <c r="I20" s="4">
+        <f>A20*(B20/1000000)^2*1000</f>
+        <v>1.0000000000000001E-7</v>
+      </c>
+      <c r="J20" s="4">
+        <f>(B$11-C20-B$12)*B20/1000</f>
+        <v>6.6999000000000008E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>100</v>
+      </c>
+      <c r="B21" s="2">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <f>B21*B$1/1000/1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="D21" s="6">
+        <f>MIN(B$16,C21*B$15*B$5)</f>
+        <v>0.37036999999999998</v>
+      </c>
+      <c r="E21" s="1">
+        <f>MIN(B$16,C21*B$15*B$6)</f>
+        <v>3.737E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>MIN(B$16,C21*B$15*B$7)</f>
+        <v>4.0699999999999998E-3</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="I21" s="4">
+        <f>A21*(B21/1000000)^2*1000</f>
+        <v>1.0000000000000003E-5</v>
+      </c>
+      <c r="J21" s="4">
+        <f>(B$11-C21-B$12)*B21/1000</f>
+        <v>6.6990000000000008E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>100</v>
+      </c>
+      <c r="B22" s="2">
+        <v>100</v>
+      </c>
+      <c r="C22">
+        <f>B22*B$1/1000/1000</f>
+        <v>0.01</v>
+      </c>
+      <c r="D22" s="6">
+        <f>MIN(B$16,C22*B$15*B$5)</f>
+        <v>3.7037</v>
+      </c>
+      <c r="E22" s="6">
+        <f>MIN(B$16,C22*B$15*B$6)</f>
+        <v>0.37370000000000003</v>
+      </c>
+      <c r="F22" s="1">
+        <f>MIN(B$16,C22*B$15*B$7)</f>
+        <v>4.07E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="I22" s="4">
+        <f>A22*(B22/1000000)^2*1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="J22" s="4">
+        <f>(B$11-C22-B$12)*B22/1000</f>
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>100</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C23">
+        <f>B23*B$1/1000/1000</f>
+        <v>0.1</v>
+      </c>
+      <c r="D23" s="7">
+        <f>MIN(B$16,C23*B$15*B$5)</f>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="E23" s="6">
+        <f>MIN(B$16,C23*B$15*B$6)</f>
+        <v>3.7369999999999997</v>
+      </c>
+      <c r="F23" s="6">
+        <f>MIN(B$16,C23*B$15*B$7)</f>
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I23" s="4">
+        <f>A23*(B23/1000000)^2*1000</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="J23" s="4">
+        <f>(B$11-C23-B$12)*B23/1000</f>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>100</v>
+      </c>
+      <c r="B24" s="2">
         <v>10000</v>
       </c>
-      <c r="B15">
-        <f>A15*B$1/1000/1000</f>
+      <c r="C24">
+        <f>B24*B$1/1000/1000</f>
         <v>1</v>
       </c>
-      <c r="C15" s="1">
-        <f>MIN(3.3,B15*10/33*B$5)</f>
-        <v>3.3</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="D24" s="7">
+        <f>MIN(B$16,C24*B$15*B$5)</f>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="E24" s="1">
+        <f>MIN(B$16,C24*B$15*B$6)</f>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="F24" s="6">
+        <f>MIN(B$16,C24*B$15*B$7)</f>
+        <v>4.07</v>
+      </c>
+      <c r="G24" s="6">
         <f t="shared" si="0"/>
-        <v>3.3</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="1"/>
-        <v>0.60606060606060608</v>
-      </c>
-      <c r="I15" s="1"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="I24" s="4">
+        <f>A24*(B24/1000000)^2*1000</f>
+        <v>10</v>
+      </c>
+      <c r="J24" s="4">
+        <f>(B$11-C24-B$12)*B24/1000</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>100</v>
+      </c>
+      <c r="B25" s="2">
         <v>50000</v>
       </c>
-      <c r="B16">
-        <f>A16*B$1/1000/1000</f>
+      <c r="C25">
+        <f>B25*B$1/1000/1000</f>
         <v>5</v>
       </c>
-      <c r="C16" s="1">
-        <f>MIN(3.3,B16*10/33*B$5)</f>
-        <v>3.3</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="D25" s="7">
+        <f>MIN(B$16,C25*B$15*B$5)</f>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="E25" s="1">
+        <f>MIN(B$16,C25*B$15*B$6)</f>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="F25" s="7">
+        <f>MIN(B$16,C25*B$15*B$7)</f>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="G25" s="6">
         <f t="shared" si="0"/>
-        <v>3.3</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="1"/>
-        <v>3.0303030303030303</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="I25" s="4">
+        <f>A25*(B25/1000000)^2*1000</f>
+        <v>250.00000000000006</v>
+      </c>
+      <c r="J25" s="4">
+        <f>(B$11-C25-B$12)*B25/1000</f>
+        <v>85.000000000000014</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2">
         <v>100000</v>
       </c>
-      <c r="B17">
-        <f>A17*B$2/1000/1000</f>
+      <c r="C26">
+        <f>B26*B$2/1000/1000</f>
         <v>5</v>
       </c>
-      <c r="C17" s="1">
-        <f>MIN(3.3,B17*10/33*B$5)</f>
-        <v>3.3</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="D26" s="7">
+        <f>MIN(B$16,C26*B$15*B$5)</f>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="E26" s="1">
+        <f>MIN(B$16,C26*B$15*B$6)</f>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="F26" s="7">
+        <f>MIN(B$16,C26*B$15*B$7)</f>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="G26" s="6">
         <f t="shared" si="0"/>
-        <v>3.3</v>
-      </c>
-      <c r="E17" s="1">
-        <f t="shared" si="1"/>
-        <v>3.0303030303030303</v>
+        <v>3.7</v>
+      </c>
+      <c r="I26" s="4">
+        <f>A26*(B26/1000000)^2*1000</f>
+        <v>500.00000000000011</v>
+      </c>
+      <c r="J26" s="4">
+        <f>(B$11-C26-B$12)*B26/1000</f>
+        <v>170.00000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Power supply voltage reduced
</commit_message>
<xml_diff>
--- a/Amplifier.xlsx
+++ b/Amplifier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\javi_\GitHub\Microwatt_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0431C2FA-5F47-4AFB-81E2-3151191C84A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7EB207-CF8B-44E6-BE9A-E6C7E3AB2F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="2130" windowWidth="17355" windowHeight="17865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17580" yWindow="2175" windowWidth="17355" windowHeight="17865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>Vout_3 (V)</t>
   </si>
   <si>
-    <t>V_ref_adc</t>
-  </si>
-  <si>
     <t>Voltage divider</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Vout_4 (V)</t>
+  </si>
+  <si>
+    <t>Vcc</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +523,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1001</v>
+        <v>1010</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>10</v>
@@ -553,7 +553,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>10</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -586,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>9</v>
@@ -598,7 +598,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>9</v>
@@ -625,7 +625,7 @@
       </c>
       <c r="B13" s="4">
         <f>B11-B12-B10</f>
-        <v>1.7000000000000002</v>
+        <v>0.70000000000000018</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>9</v>
@@ -639,20 +639,20 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4">
-        <f>3.7/B11</f>
-        <v>0.37</v>
+        <f>0.5</f>
+        <v>0.5</v>
       </c>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B16">
-        <v>4.0960000000000001</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I18" t="s">
         <v>12</v>
@@ -692,31 +692,31 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>B19*B$1/1000/1000</f>
+        <f>B19*A19/1000/1000</f>
         <v>0</v>
       </c>
       <c r="D19" s="6">
-        <f>MIN(B$16,C19*B$15*B$5)</f>
+        <f>MIN(B$16,C19*B$15*B$5+B$4)</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <f>MIN(B$16,C19*B$15*B$6+B$4)</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <f>MIN(B$16,C19*B$15*B$7+B$4)</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <f>MIN(B$16,C19*B$15*B$8+B$4)</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" ref="I19:I20" si="0">A19*(B19/1000000)^2*1000</f>
         <v>0</v>
       </c>
-      <c r="E19" s="1">
-        <f>MIN(B$16,C19*B$15*B$6)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <f>MIN(B$16,C19*B$15*B$7)</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
-        <f>MIN(B$16,C19*B$15*B$8)</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
-        <f>A19*(B19/1000000)^2*1000</f>
-        <v>0</v>
-      </c>
       <c r="J19" s="4">
-        <f>(B$11-C19-B$12)*B19/1000</f>
+        <f t="shared" ref="J19:J20" si="1">(B$11-C19-B$12)*B19/1000</f>
         <v>0</v>
       </c>
     </row>
@@ -727,33 +727,33 @@
       <c r="B20" s="2">
         <v>1</v>
       </c>
-      <c r="C20">
-        <f>B20*B$1/1000/1000</f>
+      <c r="C20" s="3">
+        <f t="shared" ref="C20:C28" si="2">B20*A20/1000/1000</f>
         <v>1E-4</v>
       </c>
       <c r="D20" s="6">
-        <f>MIN(B$16,C20*B$15*B$5)</f>
-        <v>3.7037E-2</v>
+        <f t="shared" ref="D20" si="3">MIN(B$16,C20*B$15*B$5+B$4)</f>
+        <v>1.0505</v>
       </c>
       <c r="E20" s="1">
-        <f>MIN(B$16,C20*B$15*B$6)</f>
-        <v>3.7369999999999999E-3</v>
+        <f t="shared" ref="E20" si="4">MIN(B$16,C20*B$15*B$6+B$4)</f>
+        <v>1.00505</v>
       </c>
       <c r="F20" s="1">
-        <f>MIN(B$16,C20*B$15*B$7)</f>
-        <v>4.0699999999999997E-4</v>
+        <f t="shared" ref="F20" si="5">MIN(B$16,C20*B$15*B$7+B$4)</f>
+        <v>1.0004999999999999</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" ref="G20:G26" si="0">MIN(B$16,C20*B$15*B$8)</f>
-        <v>7.3999999999999996E-5</v>
+        <f t="shared" ref="G20" si="6">MIN(B$16,C20*B$15*B$8+B$4)</f>
+        <v>1.0001</v>
       </c>
       <c r="I20" s="4">
-        <f>A20*(B20/1000000)^2*1000</f>
+        <f t="shared" si="0"/>
         <v>1.0000000000000001E-7</v>
       </c>
       <c r="J20" s="4">
-        <f>(B$11-C20-B$12)*B20/1000</f>
-        <v>6.6999000000000008E-3</v>
+        <f t="shared" si="1"/>
+        <v>3.6999000000000003E-3</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -763,33 +763,34 @@
       <c r="B21" s="2">
         <v>10</v>
       </c>
-      <c r="C21">
-        <f>B21*B$1/1000/1000</f>
+      <c r="C21" s="3">
+        <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
       <c r="D21" s="6">
-        <f>MIN(B$16,C21*B$15*B$5)</f>
-        <v>0.37036999999999998</v>
+        <f t="shared" ref="D21" si="7">MIN(B$16,C21*B$15*B$5+B$4)</f>
+        <v>1.5049999999999999</v>
       </c>
       <c r="E21" s="1">
-        <f>MIN(B$16,C21*B$15*B$6)</f>
-        <v>3.737E-2</v>
+        <f t="shared" ref="E21" si="8">MIN(B$16,C21*B$15*B$6+B$4)</f>
+        <v>1.0505</v>
       </c>
       <c r="F21" s="1">
-        <f>MIN(B$16,C21*B$15*B$7)</f>
-        <v>4.0699999999999998E-3</v>
+        <f t="shared" ref="F21" si="9">MIN(B$16,C21*B$15*B$7+B$4)</f>
+        <v>1.0049999999999999</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="0"/>
-        <v>7.3999999999999999E-4</v>
-      </c>
+        <f t="shared" ref="G21" si="10">MIN(B$16,C21*B$15*B$8+B$4)</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="H21" s="3"/>
       <c r="I21" s="4">
-        <f>A21*(B21/1000000)^2*1000</f>
+        <f t="shared" ref="I21" si="11">A21*(B21/1000000)^2*1000</f>
         <v>1.0000000000000003E-5</v>
       </c>
       <c r="J21" s="4">
-        <f>(B$11-C21-B$12)*B21/1000</f>
-        <v>6.6990000000000008E-2</v>
+        <f t="shared" ref="J21" si="12">(B$11-C21-B$12)*B21/1000</f>
+        <v>3.6989999999999995E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -797,35 +798,35 @@
         <v>100</v>
       </c>
       <c r="B22" s="2">
-        <v>100</v>
-      </c>
-      <c r="C22">
-        <f>B22*B$1/1000/1000</f>
-        <v>0.01</v>
+        <v>60</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="2"/>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D22" s="6">
-        <f>MIN(B$16,C22*B$15*B$5)</f>
-        <v>3.7037</v>
+        <f t="shared" ref="D22:D29" si="13">MIN(B$16,C22*B$15*B$5+B$4)</f>
+        <v>4.03</v>
       </c>
       <c r="E22" s="6">
-        <f>MIN(B$16,C22*B$15*B$6)</f>
-        <v>0.37370000000000003</v>
+        <f t="shared" ref="E22:E29" si="14">MIN(B$16,C22*B$15*B$6+B$4)</f>
+        <v>1.3029999999999999</v>
       </c>
       <c r="F22" s="1">
-        <f>MIN(B$16,C22*B$15*B$7)</f>
-        <v>4.07E-2</v>
+        <f t="shared" ref="F22:F29" si="15">MIN(B$16,C22*B$15*B$7+B$4)</f>
+        <v>1.03</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="0"/>
-        <v>7.4000000000000003E-3</v>
+        <f t="shared" ref="G22:G29" si="16">MIN(B$16,C22*B$15*B$8+B$4)</f>
+        <v>1.006</v>
       </c>
       <c r="I22" s="4">
-        <f>A22*(B22/1000000)^2*1000</f>
-        <v>1E-3</v>
+        <f t="shared" ref="I22:I29" si="17">A22*(B22/1000000)^2*1000</f>
+        <v>3.5999999999999997E-4</v>
       </c>
       <c r="J22" s="4">
-        <f>(B$11-C22-B$12)*B22/1000</f>
-        <v>0.66900000000000004</v>
+        <f t="shared" ref="J22:J29" si="18">(B$11-C22-B$12)*B22/1000</f>
+        <v>0.22163999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -833,35 +834,35 @@
         <v>100</v>
       </c>
       <c r="B23" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C23">
-        <f>B23*B$1/1000/1000</f>
-        <v>0.1</v>
+        <v>100</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
       </c>
       <c r="D23" s="7">
-        <f>MIN(B$16,C23*B$15*B$5)</f>
-        <v>4.0960000000000001</v>
+        <f t="shared" si="13"/>
+        <v>5</v>
       </c>
       <c r="E23" s="6">
-        <f>MIN(B$16,C23*B$15*B$6)</f>
-        <v>3.7369999999999997</v>
-      </c>
-      <c r="F23" s="6">
-        <f>MIN(B$16,C23*B$15*B$7)</f>
-        <v>0.40699999999999997</v>
+        <f t="shared" si="14"/>
+        <v>1.5049999999999999</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="15"/>
+        <v>1.05</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="0"/>
-        <v>7.3999999999999996E-2</v>
+        <f t="shared" si="16"/>
+        <v>1.01</v>
       </c>
       <c r="I23" s="4">
-        <f>A23*(B23/1000000)^2*1000</f>
-        <v>9.9999999999999992E-2</v>
+        <f t="shared" si="17"/>
+        <v>1E-3</v>
       </c>
       <c r="J23" s="4">
-        <f>(B$11-C23-B$12)*B23/1000</f>
-        <v>6.6000000000000005</v>
+        <f t="shared" si="18"/>
+        <v>0.36900000000000005</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -869,106 +870,253 @@
         <v>100</v>
       </c>
       <c r="B24" s="2">
+        <v>600</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="14"/>
+        <v>4.0299999999999994</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="15"/>
+        <v>1.3</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="16"/>
+        <v>1.06</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="4">
+        <f t="shared" si="17"/>
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="18"/>
+        <v>2.1840000000000006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>100</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="15"/>
+        <v>1.5</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="16"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="17"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="18"/>
+        <v>3.6000000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>100</v>
+      </c>
+      <c r="B26" s="2">
+        <v>6000</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="16"/>
+        <v>1.6</v>
+      </c>
+      <c r="H26" s="3"/>
+      <c r="I26" s="4">
+        <f t="shared" si="17"/>
+        <v>3.6</v>
+      </c>
+      <c r="J26" s="4">
+        <f t="shared" si="18"/>
+        <v>18.600000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>100</v>
+      </c>
+      <c r="B27" s="2">
         <v>10000</v>
       </c>
-      <c r="C24">
-        <f>B24*B$1/1000/1000</f>
+      <c r="C27" s="3">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="D24" s="7">
-        <f>MIN(B$16,C24*B$15*B$5)</f>
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="E24" s="1">
-        <f>MIN(B$16,C24*B$15*B$6)</f>
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="F24" s="6">
-        <f>MIN(B$16,C24*B$15*B$7)</f>
-        <v>4.07</v>
-      </c>
-      <c r="G24" s="6">
-        <f t="shared" si="0"/>
-        <v>0.74</v>
-      </c>
-      <c r="I24" s="4">
-        <f>A24*(B24/1000000)^2*1000</f>
+      <c r="D27" s="7">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
-      <c r="J24" s="4">
-        <f>(B$11-C24-B$12)*B24/1000</f>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="J27" s="4">
+        <f t="shared" si="18"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>100</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B28" s="2">
+        <v>20000</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="18"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29" s="2">
         <v>50000</v>
       </c>
-      <c r="C25">
-        <f>B25*B$1/1000/1000</f>
-        <v>5</v>
-      </c>
-      <c r="D25" s="7">
-        <f>MIN(B$16,C25*B$15*B$5)</f>
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="E25" s="1">
-        <f>MIN(B$16,C25*B$15*B$6)</f>
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="F25" s="7">
-        <f>MIN(B$16,C25*B$15*B$7)</f>
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="G25" s="6">
-        <f t="shared" si="0"/>
-        <v>3.7</v>
-      </c>
-      <c r="I25" s="4">
-        <f>A25*(B25/1000000)^2*1000</f>
-        <v>250.00000000000006</v>
-      </c>
-      <c r="J25" s="4">
-        <f>(B$11-C25-B$12)*B25/1000</f>
-        <v>85.000000000000014</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>50</v>
-      </c>
-      <c r="B26" s="2">
+      <c r="C29">
+        <f>B29*A29/1000/1000</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" si="17"/>
+        <v>50.000000000000007</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" si="18"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>20</v>
+      </c>
+      <c r="B30" s="2">
         <v>100000</v>
       </c>
-      <c r="C26">
-        <f>B26*B$2/1000/1000</f>
-        <v>5</v>
-      </c>
-      <c r="D26" s="7">
-        <f>MIN(B$16,C26*B$15*B$5)</f>
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="E26" s="1">
-        <f>MIN(B$16,C26*B$15*B$6)</f>
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="F26" s="7">
-        <f>MIN(B$16,C26*B$15*B$7)</f>
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="G26" s="6">
-        <f t="shared" si="0"/>
-        <v>3.7</v>
-      </c>
-      <c r="I26" s="4">
-        <f>A26*(B26/1000000)^2*1000</f>
-        <v>500.00000000000011</v>
-      </c>
-      <c r="J26" s="4">
-        <f>(B$11-C26-B$12)*B26/1000</f>
+      <c r="C30" s="3">
+        <f>B30*A30/1000/1000</f>
+        <v>2</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" ref="D30" si="19">MIN(B$16,C30*B$15*B$5+B$4)</f>
+        <v>5</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" ref="E30" si="20">MIN(B$16,C30*B$15*B$6+B$4)</f>
+        <v>5</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" ref="F30" si="21">MIN(B$16,C30*B$15*B$7+B$4)</f>
+        <v>5</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" ref="G30" si="22">MIN(B$16,C30*B$15*B$8+B$4)</f>
+        <v>3</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="4">
+        <f t="shared" ref="I30" si="23">A30*(B30/1000000)^2*1000</f>
+        <v>200.00000000000003</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" ref="J30" si="24">(B$11-C30-B$12)*B30/1000</f>
         <v>170.00000000000003</v>
       </c>
     </row>

</xml_diff>